<commit_message>
Als het goed is, is het klaar voor een nacht draaien
</commit_message>
<xml_diff>
--- a/DataSet_1.xlsx
+++ b/DataSet_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="360" windowWidth="19875" windowHeight="7710" firstSheet="33" activeTab="40"/>
+    <workbookView xWindow="480" yWindow="360" windowWidth="19875" windowHeight="7710" firstSheet="29" activeTab="40"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="18" r:id="rId1"/>
@@ -121,6 +121,609 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>6x6, k=500</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Blad15!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Blad15!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5892</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5614</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6338</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6626</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6574</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>9x4, k=500</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Blad15!$B$7:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Blad15!$E$7:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5650</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5954</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7187</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9203</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>12x3, k=500</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Blad15!$B$12:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Blad15!$E$12:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4569</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5707</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6411</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>15x2,4; k=500</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Blad15!$B$17:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Blad15!$E$17:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5337</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6462</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4543</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5332</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6840</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>6x6, k=1000</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Blad15!$B$22:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Blad15!$E$22:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>937</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1458</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1405</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1511</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>9x4, k=1000</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Blad15!$B$27:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Blad15!$E$27:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>908</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1355</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1354</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1269</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1538</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>12x3, k=1000</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Blad15!$B$32:$B$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Blad15!$E$32:$E$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1090</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>971</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1261</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1449</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>15x2,4; k=1000</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Blad15!$B$37:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Blad15!$E$37:$E$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>919</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1215</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1279</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1276</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="131974272"/>
+        <c:axId val="131975808"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="131974272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="131975808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="131975808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="131974272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafiek 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19768,8 +20371,8 @@
   <sheetPr codeName="Blad15"/>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20473,6 +21076,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>